<commit_message>
IO-fixes: FxE matrix improvements.
</commit_message>
<xml_diff>
--- a/data/zenodo_ivan/conversion/chp/CHE_convchp_biogas.xlsx
+++ b/data/zenodo_ivan/conversion/chp/CHE_convchp_biogas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo_ivan/conversion/chp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2887B0D8-02A3-7C4B-93BC-D92C1EC2DD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD2378D-4B38-D840-A1E4-CE2E1872E2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38420" yWindow="-4880" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$L$850</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$L$852</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="85">
   <si>
     <t>Name:</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t>GW/TWh</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>configuration_fxe</t>
   </si>
 </sst>
 </file>
@@ -700,11 +709,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L430"/>
+  <dimension ref="A1:L432"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -712,7 +721,7 @@
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -808,19 +817,16 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
         <v>44</v>
       </c>
       <c r="G7">
-        <v>0.24</v>
-      </c>
-      <c r="J7" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -832,19 +838,16 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
       </c>
       <c r="G8">
-        <v>0.95</v>
-      </c>
-      <c r="J8" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -856,26 +859,21 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>79</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
       </c>
       <c r="G9">
-        <v>0.25</v>
-      </c>
-      <c r="H9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" t="s">
-        <v>49</v>
+        <v>0.24</v>
       </c>
       <c r="J9" t="s">
         <v>46</v>
       </c>
-      <c r="L9" t="s">
-        <v>47</v>
-      </c>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -885,17 +883,21 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>79</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
       </c>
       <c r="G10">
-        <v>1E-3</v>
-      </c>
-      <c r="H10" t="s">
-        <v>81</v>
-      </c>
+        <v>0.95</v>
+      </c>
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -904,17 +906,17 @@
       <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
+      <c r="C11" t="s">
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>38</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
         <v>49</v>
@@ -922,7 +924,9 @@
       <c r="J11" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="L11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -931,22 +935,18 @@
       <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
+      <c r="C12" t="s">
+        <v>80</v>
       </c>
       <c r="D12" t="s">
         <v>38</v>
       </c>
       <c r="G12">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="I12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" s="2"/>
+        <v>1E-3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -956,23 +956,24 @@
         <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>38</v>
       </c>
       <c r="G13">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="I13" t="s">
+        <v>49</v>
       </c>
       <c r="J13" t="s">
-        <v>52</v>
-      </c>
-      <c r="L13" t="s">
-        <v>53</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -982,26 +983,21 @@
         <v>41</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
         <v>38</v>
       </c>
       <c r="G14">
-        <v>2.66</v>
-      </c>
-      <c r="H14" t="s">
-        <v>54</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I14" t="s">
         <v>49</v>
       </c>
       <c r="J14" t="s">
-        <v>55</v>
-      </c>
-      <c r="L14" t="s">
-        <v>56</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1011,21 +1007,23 @@
         <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
         <v>38</v>
       </c>
       <c r="G15">
-        <v>200</v>
+        <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" t="s">
-        <v>49</v>
-      </c>
-      <c r="K15" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="J15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1035,22 +1033,25 @@
         <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>38</v>
       </c>
       <c r="G16">
-        <v>0.88</v>
+        <v>2.66</v>
+      </c>
+      <c r="H16" t="s">
+        <v>54</v>
       </c>
       <c r="I16" t="s">
         <v>49</v>
       </c>
       <c r="J16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1061,23 +1062,21 @@
         <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
         <v>38</v>
       </c>
       <c r="G17">
-        <v>0.6</v>
+        <v>200</v>
+      </c>
+      <c r="H17" t="s">
+        <v>57</v>
       </c>
       <c r="I17" t="s">
         <v>49</v>
       </c>
-      <c r="J17" t="s">
-        <v>60</v>
-      </c>
-      <c r="L17" t="s">
-        <v>61</v>
-      </c>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1086,32 +1085,23 @@
       <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" t="s">
-        <v>17</v>
+      <c r="C18" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18">
-        <v>1990</v>
+        <v>38</v>
       </c>
       <c r="G18">
-        <v>80</v>
-      </c>
-      <c r="H18" t="s">
-        <v>62</v>
+        <v>0.88</v>
       </c>
       <c r="I18" t="s">
         <v>49</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="L18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1121,32 +1111,23 @@
       <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="C19" t="s">
-        <v>17</v>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19">
-        <v>1991</v>
+        <v>38</v>
       </c>
       <c r="G19">
-        <v>87</v>
-      </c>
-      <c r="H19" t="s">
-        <v>62</v>
+        <v>0.6</v>
       </c>
       <c r="I19" t="s">
         <v>49</v>
       </c>
       <c r="J19" t="s">
-        <v>63</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1163,10 +1144,10 @@
         <v>39</v>
       </c>
       <c r="E20">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="G20">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H20" t="s">
         <v>62</v>
@@ -1198,10 +1179,10 @@
         <v>39</v>
       </c>
       <c r="E21">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="G21">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="H21" t="s">
         <v>62</v>
@@ -1233,10 +1214,10 @@
         <v>39</v>
       </c>
       <c r="E22">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="G22">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="H22" t="s">
         <v>62</v>
@@ -1268,10 +1249,10 @@
         <v>39</v>
       </c>
       <c r="E23">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="G23">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="H23" t="s">
         <v>62</v>
@@ -1303,10 +1284,10 @@
         <v>39</v>
       </c>
       <c r="E24">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="G24">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="H24" t="s">
         <v>62</v>
@@ -1338,10 +1319,10 @@
         <v>39</v>
       </c>
       <c r="E25">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="G25">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H25" t="s">
         <v>62</v>
@@ -1373,10 +1354,10 @@
         <v>39</v>
       </c>
       <c r="E26">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="G26">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="H26" t="s">
         <v>62</v>
@@ -1408,10 +1389,10 @@
         <v>39</v>
       </c>
       <c r="E27">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="G27">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="H27" t="s">
         <v>62</v>
@@ -1443,10 +1424,10 @@
         <v>39</v>
       </c>
       <c r="E28">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="G28">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="H28" t="s">
         <v>62</v>
@@ -1478,10 +1459,10 @@
         <v>39</v>
       </c>
       <c r="E29">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="G29">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="H29" t="s">
         <v>62</v>
@@ -1513,10 +1494,10 @@
         <v>39</v>
       </c>
       <c r="E30">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="G30">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H30" t="s">
         <v>62</v>
@@ -1548,10 +1529,10 @@
         <v>39</v>
       </c>
       <c r="E31">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="G31">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="H31" t="s">
         <v>62</v>
@@ -1583,10 +1564,10 @@
         <v>39</v>
       </c>
       <c r="E32">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="G32">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="H32" t="s">
         <v>62</v>
@@ -1618,10 +1599,10 @@
         <v>39</v>
       </c>
       <c r="E33">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="G33">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="H33" t="s">
         <v>62</v>
@@ -1653,10 +1634,10 @@
         <v>39</v>
       </c>
       <c r="E34">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="G34">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="H34" t="s">
         <v>62</v>
@@ -1688,10 +1669,10 @@
         <v>39</v>
       </c>
       <c r="E35">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="G35">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="H35" t="s">
         <v>62</v>
@@ -1723,10 +1704,10 @@
         <v>39</v>
       </c>
       <c r="E36">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="G36">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="H36" t="s">
         <v>62</v>
@@ -1758,10 +1739,10 @@
         <v>39</v>
       </c>
       <c r="E37">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="G37">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="H37" t="s">
         <v>62</v>
@@ -1793,10 +1774,10 @@
         <v>39</v>
       </c>
       <c r="E38">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="G38">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="H38" t="s">
         <v>62</v>
@@ -1828,10 +1809,10 @@
         <v>39</v>
       </c>
       <c r="E39">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="G39">
-        <v>229</v>
+        <v>191</v>
       </c>
       <c r="H39" t="s">
         <v>62</v>
@@ -1863,10 +1844,10 @@
         <v>39</v>
       </c>
       <c r="E40">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="G40">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="H40" t="s">
         <v>62</v>
@@ -1898,10 +1879,10 @@
         <v>39</v>
       </c>
       <c r="E41">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="G41">
-        <v>279</v>
+        <v>229</v>
       </c>
       <c r="H41" t="s">
         <v>62</v>
@@ -1933,10 +1914,10 @@
         <v>39</v>
       </c>
       <c r="E42">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="G42">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="H42" t="s">
         <v>62</v>
@@ -1968,10 +1949,10 @@
         <v>39</v>
       </c>
       <c r="E43">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="G43">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="H43" t="s">
         <v>62</v>
@@ -2003,10 +1984,10 @@
         <v>39</v>
       </c>
       <c r="E44">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="G44">
-        <v>320</v>
+        <v>290</v>
       </c>
       <c r="H44" t="s">
         <v>62</v>
@@ -2038,10 +2019,10 @@
         <v>39</v>
       </c>
       <c r="E45">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="G45">
-        <v>334</v>
+        <v>303</v>
       </c>
       <c r="H45" t="s">
         <v>62</v>
@@ -2073,10 +2054,10 @@
         <v>39</v>
       </c>
       <c r="E46">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G46">
-        <v>352</v>
+        <v>320</v>
       </c>
       <c r="H46" t="s">
         <v>62</v>
@@ -2108,10 +2089,10 @@
         <v>39</v>
       </c>
       <c r="E47">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G47">
-        <v>372</v>
+        <v>334</v>
       </c>
       <c r="H47" t="s">
         <v>62</v>
@@ -2137,31 +2118,31 @@
         <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D48" t="s">
         <v>39</v>
       </c>
       <c r="E48">
-        <v>1990</v>
+        <v>2018</v>
       </c>
       <c r="G48">
-        <v>21.04945055</v>
+        <v>352</v>
       </c>
       <c r="H48" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I48" t="s">
         <v>49</v>
       </c>
       <c r="J48" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L48" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -2172,31 +2153,31 @@
         <v>41</v>
       </c>
       <c r="C49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D49" t="s">
         <v>39</v>
       </c>
       <c r="E49">
-        <v>1991</v>
+        <v>2019</v>
       </c>
       <c r="G49">
-        <v>22.33894102</v>
+        <v>372</v>
       </c>
       <c r="H49" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I49" t="s">
         <v>49</v>
       </c>
       <c r="J49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L49" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -2213,10 +2194,10 @@
         <v>39</v>
       </c>
       <c r="E50">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="G50">
-        <v>24.121794869999999</v>
+        <v>21.04945055</v>
       </c>
       <c r="H50" t="s">
         <v>57</v>
@@ -2248,10 +2229,10 @@
         <v>39</v>
       </c>
       <c r="E51">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="G51">
-        <v>28.876117319999999</v>
+        <v>22.33894102</v>
       </c>
       <c r="H51" t="s">
         <v>57</v>
@@ -2283,10 +2264,10 @@
         <v>39</v>
       </c>
       <c r="E52">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="G52">
-        <v>32.853846150000003</v>
+        <v>24.121794869999999</v>
       </c>
       <c r="H52" t="s">
         <v>57</v>
@@ -2318,10 +2299,10 @@
         <v>39</v>
       </c>
       <c r="E53">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="G53">
-        <v>34.257856670000002</v>
+        <v>28.876117319999999</v>
       </c>
       <c r="H53" t="s">
         <v>57</v>
@@ -2353,10 +2334,10 @@
         <v>39</v>
       </c>
       <c r="E54">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="G54">
-        <v>34.946620449999998</v>
+        <v>32.853846150000003</v>
       </c>
       <c r="H54" t="s">
         <v>57</v>
@@ -2388,10 +2369,10 @@
         <v>39</v>
       </c>
       <c r="E55">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="G55">
-        <v>37.418197569999997</v>
+        <v>34.257856670000002</v>
       </c>
       <c r="H55" t="s">
         <v>57</v>
@@ -2423,10 +2404,10 @@
         <v>39</v>
       </c>
       <c r="E56">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="G56">
-        <v>42.526392250000001</v>
+        <v>34.946620449999998</v>
       </c>
       <c r="H56" t="s">
         <v>57</v>
@@ -2458,10 +2439,10 @@
         <v>39</v>
       </c>
       <c r="E57">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="G57">
-        <v>42.526392250000001</v>
+        <v>37.418197569999997</v>
       </c>
       <c r="H57" t="s">
         <v>57</v>
@@ -2493,7 +2474,7 @@
         <v>39</v>
       </c>
       <c r="E58">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="G58">
         <v>42.526392250000001</v>
@@ -2528,10 +2509,10 @@
         <v>39</v>
       </c>
       <c r="E59">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="G59">
-        <v>45.701244060000001</v>
+        <v>42.526392250000001</v>
       </c>
       <c r="H59" t="s">
         <v>57</v>
@@ -2563,10 +2544,10 @@
         <v>39</v>
       </c>
       <c r="E60">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="G60">
-        <v>50.615668599999999</v>
+        <v>42.526392250000001</v>
       </c>
       <c r="H60" t="s">
         <v>57</v>
@@ -2598,10 +2579,10 @@
         <v>39</v>
       </c>
       <c r="E61">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="G61">
-        <v>50.615668599999999</v>
+        <v>45.701244060000001</v>
       </c>
       <c r="H61" t="s">
         <v>57</v>
@@ -2633,10 +2614,10 @@
         <v>39</v>
       </c>
       <c r="E62">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="G62">
-        <v>51.870777320000002</v>
+        <v>50.615668599999999</v>
       </c>
       <c r="H62" t="s">
         <v>57</v>
@@ -2668,10 +2649,10 @@
         <v>39</v>
       </c>
       <c r="E63">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="G63">
-        <v>51.870777320000002</v>
+        <v>50.615668599999999</v>
       </c>
       <c r="H63" t="s">
         <v>57</v>
@@ -2703,10 +2684,10 @@
         <v>39</v>
       </c>
       <c r="E64">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="G64">
-        <v>53.558998899999999</v>
+        <v>51.870777320000002</v>
       </c>
       <c r="H64" t="s">
         <v>57</v>
@@ -2738,10 +2719,10 @@
         <v>39</v>
       </c>
       <c r="E65">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="G65">
-        <v>53.558998899999999</v>
+        <v>51.870777320000002</v>
       </c>
       <c r="H65" t="s">
         <v>57</v>
@@ -2773,7 +2754,7 @@
         <v>39</v>
       </c>
       <c r="E66">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="G66">
         <v>53.558998899999999</v>
@@ -2808,7 +2789,7 @@
         <v>39</v>
       </c>
       <c r="E67">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="G67">
         <v>53.558998899999999</v>
@@ -2843,7 +2824,7 @@
         <v>39</v>
       </c>
       <c r="E68">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="G68">
         <v>53.558998899999999</v>
@@ -2878,7 +2859,7 @@
         <v>39</v>
       </c>
       <c r="E69">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="G69">
         <v>53.558998899999999</v>
@@ -2913,7 +2894,7 @@
         <v>39</v>
       </c>
       <c r="E70">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="G70">
         <v>53.558998899999999</v>
@@ -2948,7 +2929,7 @@
         <v>39</v>
       </c>
       <c r="E71">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="G71">
         <v>53.558998899999999</v>
@@ -2983,7 +2964,7 @@
         <v>39</v>
       </c>
       <c r="E72">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="G72">
         <v>53.558998899999999</v>
@@ -3018,7 +2999,7 @@
         <v>39</v>
       </c>
       <c r="E73">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="G73">
         <v>53.558998899999999</v>
@@ -3053,7 +3034,7 @@
         <v>39</v>
       </c>
       <c r="E74">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="G74">
         <v>53.558998899999999</v>
@@ -3088,10 +3069,10 @@
         <v>39</v>
       </c>
       <c r="E75">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="G75">
-        <v>56.087386670000001</v>
+        <v>53.558998899999999</v>
       </c>
       <c r="H75" t="s">
         <v>57</v>
@@ -3123,10 +3104,10 @@
         <v>39</v>
       </c>
       <c r="E76">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G76">
-        <v>60.844335350000001</v>
+        <v>53.558998899999999</v>
       </c>
       <c r="H76" t="s">
         <v>57</v>
@@ -3158,10 +3139,10 @@
         <v>39</v>
       </c>
       <c r="E77">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G77">
-        <v>60.844335350000001</v>
+        <v>56.087386670000001</v>
       </c>
       <c r="H77" t="s">
         <v>57</v>
@@ -3187,16 +3168,16 @@
         <v>41</v>
       </c>
       <c r="C78" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D78" t="s">
         <v>39</v>
       </c>
       <c r="E78">
-        <v>1990</v>
+        <v>2018</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>60.844335350000001</v>
       </c>
       <c r="H78" t="s">
         <v>57</v>
@@ -3207,8 +3188,11 @@
       <c r="J78" t="s">
         <v>66</v>
       </c>
+      <c r="K78" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="L78" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
@@ -3219,16 +3203,16 @@
         <v>41</v>
       </c>
       <c r="C79" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D79" t="s">
         <v>39</v>
       </c>
       <c r="E79">
-        <v>1991</v>
+        <v>2019</v>
       </c>
       <c r="G79">
-        <v>1.289490469</v>
+        <v>60.844335350000001</v>
       </c>
       <c r="H79" t="s">
         <v>57</v>
@@ -3239,8 +3223,11 @@
       <c r="J79" t="s">
         <v>66</v>
       </c>
+      <c r="K79" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="L79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
@@ -3257,10 +3244,10 @@
         <v>39</v>
       </c>
       <c r="E80">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="G80">
-        <v>1.782853853</v>
+        <v>0</v>
       </c>
       <c r="H80" t="s">
         <v>57</v>
@@ -3289,10 +3276,10 @@
         <v>39</v>
       </c>
       <c r="E81">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="G81">
-        <v>4.7543224469999998</v>
+        <v>1.289490469</v>
       </c>
       <c r="H81" t="s">
         <v>57</v>
@@ -3321,10 +3308,10 @@
         <v>39</v>
       </c>
       <c r="E82">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="G82">
-        <v>3.9777288350000002</v>
+        <v>1.782853853</v>
       </c>
       <c r="H82" t="s">
         <v>57</v>
@@ -3353,10 +3340,10 @@
         <v>39</v>
       </c>
       <c r="E83">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="G83">
-        <v>1.4040105190000001</v>
+        <v>4.7543224469999998</v>
       </c>
       <c r="H83" t="s">
         <v>57</v>
@@ -3385,10 +3372,10 @@
         <v>39</v>
       </c>
       <c r="E84">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="G84">
-        <v>0.68876377700000002</v>
+        <v>3.9777288350000002</v>
       </c>
       <c r="H84" t="s">
         <v>57</v>
@@ -3417,10 +3404,10 @@
         <v>39</v>
       </c>
       <c r="E85">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="G85">
-        <v>2.4715771229999999</v>
+        <v>1.4040105190000001</v>
       </c>
       <c r="H85" t="s">
         <v>57</v>
@@ -3449,10 +3436,10 @@
         <v>39</v>
       </c>
       <c r="E86">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="G86">
-        <v>5.1081946780000003</v>
+        <v>0.68876377700000002</v>
       </c>
       <c r="H86" t="s">
         <v>57</v>
@@ -3481,10 +3468,10 @@
         <v>39</v>
       </c>
       <c r="E87">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>2.4715771229999999</v>
       </c>
       <c r="H87" t="s">
         <v>57</v>
@@ -3513,10 +3500,10 @@
         <v>39</v>
       </c>
       <c r="E88">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>5.1081946780000003</v>
       </c>
       <c r="H88" t="s">
         <v>57</v>
@@ -3545,10 +3532,10 @@
         <v>39</v>
       </c>
       <c r="E89">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="G89">
-        <v>3.1748518040000002</v>
+        <v>0</v>
       </c>
       <c r="H89" t="s">
         <v>57</v>
@@ -3577,10 +3564,10 @@
         <v>39</v>
       </c>
       <c r="E90">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="G90">
-        <v>4.9144245419999999</v>
+        <v>0</v>
       </c>
       <c r="H90" t="s">
         <v>57</v>
@@ -3609,10 +3596,10 @@
         <v>39</v>
       </c>
       <c r="E91">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>3.1748518040000002</v>
       </c>
       <c r="H91" t="s">
         <v>57</v>
@@ -3641,10 +3628,10 @@
         <v>39</v>
       </c>
       <c r="E92">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="G92">
-        <v>1.2551087249999999</v>
+        <v>4.9144245419999999</v>
       </c>
       <c r="H92" t="s">
         <v>57</v>
@@ -3673,7 +3660,7 @@
         <v>39</v>
       </c>
       <c r="E93">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -3705,10 +3692,10 @@
         <v>39</v>
       </c>
       <c r="E94">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="G94">
-        <v>1.6882215780000001</v>
+        <v>1.2551087249999999</v>
       </c>
       <c r="H94" t="s">
         <v>57</v>
@@ -3737,7 +3724,7 @@
         <v>39</v>
       </c>
       <c r="E95">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -3769,10 +3756,10 @@
         <v>39</v>
       </c>
       <c r="E96">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>1.6882215780000001</v>
       </c>
       <c r="H96" t="s">
         <v>57</v>
@@ -3801,7 +3788,7 @@
         <v>39</v>
       </c>
       <c r="E97">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -3833,7 +3820,7 @@
         <v>39</v>
       </c>
       <c r="E98">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -3865,7 +3852,7 @@
         <v>39</v>
       </c>
       <c r="E99">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -3897,7 +3884,7 @@
         <v>39</v>
       </c>
       <c r="E100">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -3929,7 +3916,7 @@
         <v>39</v>
       </c>
       <c r="E101">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -3961,7 +3948,7 @@
         <v>39</v>
       </c>
       <c r="E102">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -3993,7 +3980,7 @@
         <v>39</v>
       </c>
       <c r="E103">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4025,7 +4012,7 @@
         <v>39</v>
       </c>
       <c r="E104">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -4057,10 +4044,10 @@
         <v>39</v>
       </c>
       <c r="E105">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="G105">
-        <v>2.5283877709999998</v>
+        <v>0</v>
       </c>
       <c r="H105" t="s">
         <v>57</v>
@@ -4089,10 +4076,10 @@
         <v>39</v>
       </c>
       <c r="E106">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G106">
-        <v>4.756948682</v>
+        <v>0</v>
       </c>
       <c r="H106" t="s">
         <v>57</v>
@@ -4121,10 +4108,10 @@
         <v>39</v>
       </c>
       <c r="E107">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G107">
-        <v>0</v>
+        <v>2.5283877709999998</v>
       </c>
       <c r="H107" t="s">
         <v>57</v>
@@ -4147,16 +4134,16 @@
         <v>41</v>
       </c>
       <c r="C108" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D108" t="s">
         <v>39</v>
       </c>
       <c r="E108">
-        <v>1990</v>
+        <v>2018</v>
       </c>
       <c r="G108">
-        <v>0</v>
+        <v>4.756948682</v>
       </c>
       <c r="H108" t="s">
         <v>57</v>
@@ -4179,13 +4166,13 @@
         <v>41</v>
       </c>
       <c r="C109" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D109" t="s">
         <v>39</v>
       </c>
       <c r="E109">
-        <v>1991</v>
+        <v>2019</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -4217,7 +4204,7 @@
         <v>39</v>
       </c>
       <c r="E110">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -4249,7 +4236,7 @@
         <v>39</v>
       </c>
       <c r="E111">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -4281,7 +4268,7 @@
         <v>39</v>
       </c>
       <c r="E112">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -4313,7 +4300,7 @@
         <v>39</v>
       </c>
       <c r="E113">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -4345,7 +4332,7 @@
         <v>39</v>
       </c>
       <c r="E114">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -4377,7 +4364,7 @@
         <v>39</v>
       </c>
       <c r="E115">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -4409,7 +4396,7 @@
         <v>39</v>
       </c>
       <c r="E116">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -4441,7 +4428,7 @@
         <v>39</v>
       </c>
       <c r="E117">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -4473,7 +4460,7 @@
         <v>39</v>
       </c>
       <c r="E118">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -4505,7 +4492,7 @@
         <v>39</v>
       </c>
       <c r="E119">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -4537,7 +4524,7 @@
         <v>39</v>
       </c>
       <c r="E120">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -4569,7 +4556,7 @@
         <v>39</v>
       </c>
       <c r="E121">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -4601,7 +4588,7 @@
         <v>39</v>
       </c>
       <c r="E122">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -4633,7 +4620,7 @@
         <v>39</v>
       </c>
       <c r="E123">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -4665,7 +4652,7 @@
         <v>39</v>
       </c>
       <c r="E124">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -4697,7 +4684,7 @@
         <v>39</v>
       </c>
       <c r="E125">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -4729,7 +4716,7 @@
         <v>39</v>
       </c>
       <c r="E126">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -4761,7 +4748,7 @@
         <v>39</v>
       </c>
       <c r="E127">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="G127">
         <v>0</v>
@@ -4793,7 +4780,7 @@
         <v>39</v>
       </c>
       <c r="E128">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="G128">
         <v>0</v>
@@ -4825,7 +4812,7 @@
         <v>39</v>
       </c>
       <c r="E129">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="G129">
         <v>0</v>
@@ -4857,7 +4844,7 @@
         <v>39</v>
       </c>
       <c r="E130">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="G130">
         <v>0</v>
@@ -4889,7 +4876,7 @@
         <v>39</v>
       </c>
       <c r="E131">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="G131">
         <v>0</v>
@@ -4921,7 +4908,7 @@
         <v>39</v>
       </c>
       <c r="E132">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="G132">
         <v>0</v>
@@ -4953,7 +4940,7 @@
         <v>39</v>
       </c>
       <c r="E133">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="G133">
         <v>0</v>
@@ -4985,7 +4972,7 @@
         <v>39</v>
       </c>
       <c r="E134">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="G134">
         <v>0</v>
@@ -5017,7 +5004,7 @@
         <v>39</v>
       </c>
       <c r="E135">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="G135">
         <v>0</v>
@@ -5049,7 +5036,7 @@
         <v>39</v>
       </c>
       <c r="E136">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G136">
         <v>0</v>
@@ -5081,7 +5068,7 @@
         <v>39</v>
       </c>
       <c r="E137">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G137">
         <v>0</v>
@@ -5107,16 +5094,28 @@
         <v>41</v>
       </c>
       <c r="C138" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D138" t="s">
         <v>39</v>
       </c>
       <c r="E138">
-        <v>1990</v>
+        <v>2018</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+      <c r="H138" t="s">
+        <v>57</v>
       </c>
       <c r="I138" t="s">
         <v>49</v>
+      </c>
+      <c r="J138" t="s">
+        <v>66</v>
+      </c>
+      <c r="L138" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.2">
@@ -5127,16 +5126,28 @@
         <v>41</v>
       </c>
       <c r="C139" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D139" t="s">
         <v>39</v>
       </c>
       <c r="E139">
-        <v>1991</v>
+        <v>2019</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+      <c r="H139" t="s">
+        <v>57</v>
       </c>
       <c r="I139" t="s">
         <v>49</v>
+      </c>
+      <c r="J139" t="s">
+        <v>66</v>
+      </c>
+      <c r="L139" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.2">
@@ -5153,7 +5164,7 @@
         <v>39</v>
       </c>
       <c r="E140">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="I140" t="s">
         <v>49</v>
@@ -5173,7 +5184,7 @@
         <v>39</v>
       </c>
       <c r="E141">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="I141" t="s">
         <v>49</v>
@@ -5193,7 +5204,7 @@
         <v>39</v>
       </c>
       <c r="E142">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="I142" t="s">
         <v>49</v>
@@ -5213,7 +5224,7 @@
         <v>39</v>
       </c>
       <c r="E143">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="I143" t="s">
         <v>49</v>
@@ -5233,7 +5244,7 @@
         <v>39</v>
       </c>
       <c r="E144">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="I144" t="s">
         <v>49</v>
@@ -5253,7 +5264,7 @@
         <v>39</v>
       </c>
       <c r="E145">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="I145" t="s">
         <v>49</v>
@@ -5273,7 +5284,7 @@
         <v>39</v>
       </c>
       <c r="E146">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="I146" t="s">
         <v>49</v>
@@ -5293,7 +5304,7 @@
         <v>39</v>
       </c>
       <c r="E147">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="I147" t="s">
         <v>49</v>
@@ -5313,7 +5324,7 @@
         <v>39</v>
       </c>
       <c r="E148">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="I148" t="s">
         <v>49</v>
@@ -5333,7 +5344,7 @@
         <v>39</v>
       </c>
       <c r="E149">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="I149" t="s">
         <v>49</v>
@@ -5353,7 +5364,7 @@
         <v>39</v>
       </c>
       <c r="E150">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="I150" t="s">
         <v>49</v>
@@ -5373,7 +5384,7 @@
         <v>39</v>
       </c>
       <c r="E151">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="I151" t="s">
         <v>49</v>
@@ -5393,7 +5404,7 @@
         <v>39</v>
       </c>
       <c r="E152">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="I152" t="s">
         <v>49</v>
@@ -5413,7 +5424,7 @@
         <v>39</v>
       </c>
       <c r="E153">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="I153" t="s">
         <v>49</v>
@@ -5433,7 +5444,7 @@
         <v>39</v>
       </c>
       <c r="E154">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="I154" t="s">
         <v>49</v>
@@ -5453,7 +5464,7 @@
         <v>39</v>
       </c>
       <c r="E155">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="I155" t="s">
         <v>49</v>
@@ -5473,7 +5484,7 @@
         <v>39</v>
       </c>
       <c r="E156">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="I156" t="s">
         <v>49</v>
@@ -5493,7 +5504,7 @@
         <v>39</v>
       </c>
       <c r="E157">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="I157" t="s">
         <v>49</v>
@@ -5513,7 +5524,7 @@
         <v>39</v>
       </c>
       <c r="E158">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="I158" t="s">
         <v>49</v>
@@ -5533,7 +5544,7 @@
         <v>39</v>
       </c>
       <c r="E159">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="I159" t="s">
         <v>49</v>
@@ -5553,7 +5564,7 @@
         <v>39</v>
       </c>
       <c r="E160">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="I160" t="s">
         <v>49</v>
@@ -5573,7 +5584,7 @@
         <v>39</v>
       </c>
       <c r="E161">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="I161" t="s">
         <v>49</v>
@@ -5593,7 +5604,7 @@
         <v>39</v>
       </c>
       <c r="E162">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="I162" t="s">
         <v>49</v>
@@ -5613,7 +5624,7 @@
         <v>39</v>
       </c>
       <c r="E163">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="I163" t="s">
         <v>49</v>
@@ -5633,7 +5644,7 @@
         <v>39</v>
       </c>
       <c r="E164">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="I164" t="s">
         <v>49</v>
@@ -5653,7 +5664,7 @@
         <v>39</v>
       </c>
       <c r="E165">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="I165" t="s">
         <v>49</v>
@@ -5673,22 +5684,10 @@
         <v>39</v>
       </c>
       <c r="E166">
-        <v>2018</v>
-      </c>
-      <c r="G166">
-        <v>538</v>
-      </c>
-      <c r="H166" t="s">
-        <v>70</v>
+        <v>2016</v>
       </c>
       <c r="I166" t="s">
         <v>49</v>
-      </c>
-      <c r="J166" t="s">
-        <v>52</v>
-      </c>
-      <c r="L166" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.2">
@@ -5705,7 +5704,7 @@
         <v>39</v>
       </c>
       <c r="E167">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="I167" t="s">
         <v>49</v>
@@ -5719,16 +5718,28 @@
         <v>41</v>
       </c>
       <c r="C168" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D168" t="s">
         <v>39</v>
       </c>
       <c r="E168">
-        <v>1990</v>
+        <v>2018</v>
+      </c>
+      <c r="G168">
+        <v>538</v>
+      </c>
+      <c r="H168" t="s">
+        <v>70</v>
       </c>
       <c r="I168" t="s">
         <v>49</v>
+      </c>
+      <c r="J168" t="s">
+        <v>52</v>
+      </c>
+      <c r="L168" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.2">
@@ -5739,13 +5750,13 @@
         <v>41</v>
       </c>
       <c r="C169" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D169" t="s">
         <v>39</v>
       </c>
       <c r="E169">
-        <v>1991</v>
+        <v>2019</v>
       </c>
       <c r="I169" t="s">
         <v>49</v>
@@ -5765,7 +5776,7 @@
         <v>39</v>
       </c>
       <c r="E170">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="I170" t="s">
         <v>49</v>
@@ -5785,7 +5796,7 @@
         <v>39</v>
       </c>
       <c r="E171">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="I171" t="s">
         <v>49</v>
@@ -5805,7 +5816,7 @@
         <v>39</v>
       </c>
       <c r="E172">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="I172" t="s">
         <v>49</v>
@@ -5825,7 +5836,7 @@
         <v>39</v>
       </c>
       <c r="E173">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="I173" t="s">
         <v>49</v>
@@ -5845,7 +5856,7 @@
         <v>39</v>
       </c>
       <c r="E174">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="I174" t="s">
         <v>49</v>
@@ -5865,7 +5876,7 @@
         <v>39</v>
       </c>
       <c r="E175">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="I175" t="s">
         <v>49</v>
@@ -5885,7 +5896,7 @@
         <v>39</v>
       </c>
       <c r="E176">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="I176" t="s">
         <v>49</v>
@@ -5905,7 +5916,7 @@
         <v>39</v>
       </c>
       <c r="E177">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="I177" t="s">
         <v>49</v>
@@ -5925,7 +5936,7 @@
         <v>39</v>
       </c>
       <c r="E178">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="I178" t="s">
         <v>49</v>
@@ -5945,7 +5956,7 @@
         <v>39</v>
       </c>
       <c r="E179">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="I179" t="s">
         <v>49</v>
@@ -5965,7 +5976,7 @@
         <v>39</v>
       </c>
       <c r="E180">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="I180" t="s">
         <v>49</v>
@@ -5985,7 +5996,7 @@
         <v>39</v>
       </c>
       <c r="E181">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="I181" t="s">
         <v>49</v>
@@ -6005,7 +6016,7 @@
         <v>39</v>
       </c>
       <c r="E182">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="I182" t="s">
         <v>49</v>
@@ -6025,7 +6036,7 @@
         <v>39</v>
       </c>
       <c r="E183">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="I183" t="s">
         <v>49</v>
@@ -6045,7 +6056,7 @@
         <v>39</v>
       </c>
       <c r="E184">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="I184" t="s">
         <v>49</v>
@@ -6065,7 +6076,7 @@
         <v>39</v>
       </c>
       <c r="E185">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="I185" t="s">
         <v>49</v>
@@ -6085,7 +6096,7 @@
         <v>39</v>
       </c>
       <c r="E186">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="I186" t="s">
         <v>49</v>
@@ -6105,7 +6116,7 @@
         <v>39</v>
       </c>
       <c r="E187">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="I187" t="s">
         <v>49</v>
@@ -6125,7 +6136,7 @@
         <v>39</v>
       </c>
       <c r="E188">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="I188" t="s">
         <v>49</v>
@@ -6145,7 +6156,7 @@
         <v>39</v>
       </c>
       <c r="E189">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="I189" t="s">
         <v>49</v>
@@ -6165,7 +6176,7 @@
         <v>39</v>
       </c>
       <c r="E190">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="I190" t="s">
         <v>49</v>
@@ -6185,7 +6196,7 @@
         <v>39</v>
       </c>
       <c r="E191">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="I191" t="s">
         <v>49</v>
@@ -6205,7 +6216,7 @@
         <v>39</v>
       </c>
       <c r="E192">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="I192" t="s">
         <v>49</v>
@@ -6225,7 +6236,7 @@
         <v>39</v>
       </c>
       <c r="E193">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="I193" t="s">
         <v>49</v>
@@ -6245,7 +6256,7 @@
         <v>39</v>
       </c>
       <c r="E194">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="I194" t="s">
         <v>49</v>
@@ -6265,7 +6276,7 @@
         <v>39</v>
       </c>
       <c r="E195">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="I195" t="s">
         <v>49</v>
@@ -6285,22 +6296,10 @@
         <v>39</v>
       </c>
       <c r="E196">
-        <v>2018</v>
-      </c>
-      <c r="G196">
-        <v>9532</v>
-      </c>
-      <c r="H196" t="s">
-        <v>70</v>
+        <v>2016</v>
       </c>
       <c r="I196" t="s">
         <v>49</v>
-      </c>
-      <c r="J196" t="s">
-        <v>52</v>
-      </c>
-      <c r="L196" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.2">
@@ -6317,7 +6316,7 @@
         <v>39</v>
       </c>
       <c r="E197">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="I197" t="s">
         <v>49</v>
@@ -6331,16 +6330,28 @@
         <v>41</v>
       </c>
       <c r="C198" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D198" t="s">
         <v>39</v>
       </c>
       <c r="E198">
-        <v>1990</v>
+        <v>2018</v>
+      </c>
+      <c r="G198">
+        <v>9532</v>
+      </c>
+      <c r="H198" t="s">
+        <v>70</v>
       </c>
       <c r="I198" t="s">
         <v>49</v>
+      </c>
+      <c r="J198" t="s">
+        <v>52</v>
+      </c>
+      <c r="L198" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.2">
@@ -6351,13 +6362,13 @@
         <v>41</v>
       </c>
       <c r="C199" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D199" t="s">
         <v>39</v>
       </c>
       <c r="E199">
-        <v>1991</v>
+        <v>2019</v>
       </c>
       <c r="I199" t="s">
         <v>49</v>
@@ -6377,7 +6388,7 @@
         <v>39</v>
       </c>
       <c r="E200">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="I200" t="s">
         <v>49</v>
@@ -6397,7 +6408,7 @@
         <v>39</v>
       </c>
       <c r="E201">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="I201" t="s">
         <v>49</v>
@@ -6417,7 +6428,7 @@
         <v>39</v>
       </c>
       <c r="E202">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="I202" t="s">
         <v>49</v>
@@ -6437,7 +6448,7 @@
         <v>39</v>
       </c>
       <c r="E203">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="I203" t="s">
         <v>49</v>
@@ -6457,7 +6468,7 @@
         <v>39</v>
       </c>
       <c r="E204">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="I204" t="s">
         <v>49</v>
@@ -6477,7 +6488,7 @@
         <v>39</v>
       </c>
       <c r="E205">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="I205" t="s">
         <v>49</v>
@@ -6497,7 +6508,7 @@
         <v>39</v>
       </c>
       <c r="E206">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="I206" t="s">
         <v>49</v>
@@ -6517,7 +6528,7 @@
         <v>39</v>
       </c>
       <c r="E207">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="I207" t="s">
         <v>49</v>
@@ -6537,7 +6548,7 @@
         <v>39</v>
       </c>
       <c r="E208">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="I208" t="s">
         <v>49</v>
@@ -6557,7 +6568,7 @@
         <v>39</v>
       </c>
       <c r="E209">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="I209" t="s">
         <v>49</v>
@@ -6577,7 +6588,7 @@
         <v>39</v>
       </c>
       <c r="E210">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="I210" t="s">
         <v>49</v>
@@ -6597,7 +6608,7 @@
         <v>39</v>
       </c>
       <c r="E211">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="I211" t="s">
         <v>49</v>
@@ -6617,7 +6628,7 @@
         <v>39</v>
       </c>
       <c r="E212">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="I212" t="s">
         <v>49</v>
@@ -6637,7 +6648,7 @@
         <v>39</v>
       </c>
       <c r="E213">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="I213" t="s">
         <v>49</v>
@@ -6657,7 +6668,7 @@
         <v>39</v>
       </c>
       <c r="E214">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="I214" t="s">
         <v>49</v>
@@ -6677,7 +6688,7 @@
         <v>39</v>
       </c>
       <c r="E215">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="I215" t="s">
         <v>49</v>
@@ -6697,7 +6708,7 @@
         <v>39</v>
       </c>
       <c r="E216">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="I216" t="s">
         <v>49</v>
@@ -6717,7 +6728,7 @@
         <v>39</v>
       </c>
       <c r="E217">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="I217" t="s">
         <v>49</v>
@@ -6737,7 +6748,7 @@
         <v>39</v>
       </c>
       <c r="E218">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="I218" t="s">
         <v>49</v>
@@ -6757,7 +6768,7 @@
         <v>39</v>
       </c>
       <c r="E219">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="I219" t="s">
         <v>49</v>
@@ -6777,7 +6788,7 @@
         <v>39</v>
       </c>
       <c r="E220">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="I220" t="s">
         <v>49</v>
@@ -6797,7 +6808,7 @@
         <v>39</v>
       </c>
       <c r="E221">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="I221" t="s">
         <v>49</v>
@@ -6817,7 +6828,7 @@
         <v>39</v>
       </c>
       <c r="E222">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="I222" t="s">
         <v>49</v>
@@ -6837,7 +6848,7 @@
         <v>39</v>
       </c>
       <c r="E223">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="I223" t="s">
         <v>49</v>
@@ -6857,7 +6868,7 @@
         <v>39</v>
       </c>
       <c r="E224">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="I224" t="s">
         <v>49</v>
@@ -6877,7 +6888,7 @@
         <v>39</v>
       </c>
       <c r="E225">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="I225" t="s">
         <v>49</v>
@@ -6897,22 +6908,10 @@
         <v>39</v>
       </c>
       <c r="E226">
-        <v>2018</v>
-      </c>
-      <c r="G226">
-        <v>0</v>
-      </c>
-      <c r="H226" t="s">
-        <v>73</v>
+        <v>2016</v>
       </c>
       <c r="I226" t="s">
         <v>49</v>
-      </c>
-      <c r="J226" t="s">
-        <v>52</v>
-      </c>
-      <c r="L226" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.2">
@@ -6929,7 +6928,7 @@
         <v>39</v>
       </c>
       <c r="E227">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="I227" t="s">
         <v>49</v>
@@ -6943,28 +6942,28 @@
         <v>41</v>
       </c>
       <c r="C228" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D228" t="s">
         <v>39</v>
       </c>
       <c r="E228">
-        <v>1990</v>
+        <v>2018</v>
       </c>
       <c r="G228">
         <v>0</v>
       </c>
       <c r="H228" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="I228" t="s">
         <v>49</v>
       </c>
       <c r="J228" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="L228" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
@@ -6975,28 +6974,16 @@
         <v>41</v>
       </c>
       <c r="C229" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D229" t="s">
         <v>39</v>
       </c>
       <c r="E229">
-        <v>1991</v>
-      </c>
-      <c r="G229">
-        <v>0</v>
-      </c>
-      <c r="H229" t="s">
-        <v>57</v>
+        <v>2019</v>
       </c>
       <c r="I229" t="s">
         <v>49</v>
-      </c>
-      <c r="J229" t="s">
-        <v>66</v>
-      </c>
-      <c r="L229" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.2">
@@ -7013,7 +7000,7 @@
         <v>39</v>
       </c>
       <c r="E230">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="G230">
         <v>0</v>
@@ -7045,7 +7032,7 @@
         <v>39</v>
       </c>
       <c r="E231">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="G231">
         <v>0</v>
@@ -7077,7 +7064,7 @@
         <v>39</v>
       </c>
       <c r="E232">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="G232">
         <v>0</v>
@@ -7109,7 +7096,7 @@
         <v>39</v>
       </c>
       <c r="E233">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="G233">
         <v>0</v>
@@ -7141,7 +7128,7 @@
         <v>39</v>
       </c>
       <c r="E234">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="G234">
         <v>0</v>
@@ -7173,7 +7160,7 @@
         <v>39</v>
       </c>
       <c r="E235">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="G235">
         <v>0</v>
@@ -7205,7 +7192,7 @@
         <v>39</v>
       </c>
       <c r="E236">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="G236">
         <v>0</v>
@@ -7237,7 +7224,7 @@
         <v>39</v>
       </c>
       <c r="E237">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="G237">
         <v>0</v>
@@ -7269,7 +7256,7 @@
         <v>39</v>
       </c>
       <c r="E238">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="G238">
         <v>0</v>
@@ -7301,7 +7288,7 @@
         <v>39</v>
       </c>
       <c r="E239">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="G239">
         <v>0</v>
@@ -7333,7 +7320,7 @@
         <v>39</v>
       </c>
       <c r="E240">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="G240">
         <v>0</v>
@@ -7365,7 +7352,7 @@
         <v>39</v>
       </c>
       <c r="E241">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="G241">
         <v>0</v>
@@ -7397,7 +7384,7 @@
         <v>39</v>
       </c>
       <c r="E242">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="G242">
         <v>0</v>
@@ -7429,7 +7416,7 @@
         <v>39</v>
       </c>
       <c r="E243">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="G243">
         <v>0</v>
@@ -7461,7 +7448,7 @@
         <v>39</v>
       </c>
       <c r="E244">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="G244">
         <v>0</v>
@@ -7493,7 +7480,7 @@
         <v>39</v>
       </c>
       <c r="E245">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="G245">
         <v>0</v>
@@ -7525,7 +7512,7 @@
         <v>39</v>
       </c>
       <c r="E246">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="G246">
         <v>0</v>
@@ -7557,7 +7544,7 @@
         <v>39</v>
       </c>
       <c r="E247">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="G247">
         <v>0</v>
@@ -7589,7 +7576,7 @@
         <v>39</v>
       </c>
       <c r="E248">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="G248">
         <v>0</v>
@@ -7621,7 +7608,7 @@
         <v>39</v>
       </c>
       <c r="E249">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="G249">
         <v>0</v>
@@ -7653,7 +7640,7 @@
         <v>39</v>
       </c>
       <c r="E250">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="G250">
         <v>0</v>
@@ -7685,7 +7672,7 @@
         <v>39</v>
       </c>
       <c r="E251">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="G251">
         <v>0</v>
@@ -7717,7 +7704,7 @@
         <v>39</v>
       </c>
       <c r="E252">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="G252">
         <v>0</v>
@@ -7749,7 +7736,7 @@
         <v>39</v>
       </c>
       <c r="E253">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="G253">
         <v>0</v>
@@ -7781,7 +7768,7 @@
         <v>39</v>
       </c>
       <c r="E254">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="G254">
         <v>0</v>
@@ -7813,7 +7800,7 @@
         <v>39</v>
       </c>
       <c r="E255">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -7845,7 +7832,7 @@
         <v>39</v>
       </c>
       <c r="E256">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G256">
         <v>0</v>
@@ -7877,7 +7864,7 @@
         <v>39</v>
       </c>
       <c r="E257">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G257">
         <v>0</v>
@@ -7903,28 +7890,28 @@
         <v>41</v>
       </c>
       <c r="C258" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D258" t="s">
         <v>39</v>
       </c>
       <c r="E258">
-        <v>1990</v>
+        <v>2018</v>
       </c>
       <c r="G258">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H258" t="s">
+        <v>57</v>
       </c>
       <c r="I258" t="s">
         <v>49</v>
       </c>
       <c r="J258" t="s">
-        <v>76</v>
-      </c>
-      <c r="K258" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="L258" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.2">
@@ -7935,19 +7922,28 @@
         <v>41</v>
       </c>
       <c r="C259" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D259" t="s">
         <v>39</v>
       </c>
       <c r="E259">
-        <v>1991</v>
+        <v>2019</v>
       </c>
       <c r="G259">
-        <v>0.85</v>
+        <v>0</v>
+      </c>
+      <c r="H259" t="s">
+        <v>57</v>
       </c>
       <c r="I259" t="s">
         <v>49</v>
+      </c>
+      <c r="J259" t="s">
+        <v>66</v>
+      </c>
+      <c r="L259" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.2">
@@ -7964,13 +7960,22 @@
         <v>39</v>
       </c>
       <c r="E260">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="G260">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="I260" t="s">
         <v>49</v>
+      </c>
+      <c r="J260" t="s">
+        <v>76</v>
+      </c>
+      <c r="K260" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L260" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.2">
@@ -7987,7 +7992,7 @@
         <v>39</v>
       </c>
       <c r="E261">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="G261">
         <v>0.85</v>
@@ -8010,7 +8015,7 @@
         <v>39</v>
       </c>
       <c r="E262">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="G262">
         <v>0.85</v>
@@ -8033,7 +8038,7 @@
         <v>39</v>
       </c>
       <c r="E263">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="G263">
         <v>0.85</v>
@@ -8056,7 +8061,7 @@
         <v>39</v>
       </c>
       <c r="E264">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="G264">
         <v>0.85</v>
@@ -8079,7 +8084,7 @@
         <v>39</v>
       </c>
       <c r="E265">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="G265">
         <v>0.85</v>
@@ -8102,7 +8107,7 @@
         <v>39</v>
       </c>
       <c r="E266">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="G266">
         <v>0.85</v>
@@ -8125,7 +8130,7 @@
         <v>39</v>
       </c>
       <c r="E267">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="G267">
         <v>0.85</v>
@@ -8148,7 +8153,7 @@
         <v>39</v>
       </c>
       <c r="E268">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="G268">
         <v>0.85</v>
@@ -8171,7 +8176,7 @@
         <v>39</v>
       </c>
       <c r="E269">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="G269">
         <v>0.85</v>
@@ -8194,7 +8199,7 @@
         <v>39</v>
       </c>
       <c r="E270">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="G270">
         <v>0.85</v>
@@ -8217,7 +8222,7 @@
         <v>39</v>
       </c>
       <c r="E271">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="G271">
         <v>0.85</v>
@@ -8240,7 +8245,7 @@
         <v>39</v>
       </c>
       <c r="E272">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="G272">
         <v>0.85</v>
@@ -8263,7 +8268,7 @@
         <v>39</v>
       </c>
       <c r="E273">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="G273">
         <v>0.85</v>
@@ -8286,7 +8291,7 @@
         <v>39</v>
       </c>
       <c r="E274">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="G274">
         <v>0.85</v>
@@ -8309,7 +8314,7 @@
         <v>39</v>
       </c>
       <c r="E275">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="G275">
         <v>0.85</v>
@@ -8332,7 +8337,7 @@
         <v>39</v>
       </c>
       <c r="E276">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="G276">
         <v>0.85</v>
@@ -8355,7 +8360,7 @@
         <v>39</v>
       </c>
       <c r="E277">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="G277">
         <v>0.85</v>
@@ -8378,7 +8383,7 @@
         <v>39</v>
       </c>
       <c r="E278">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="G278">
         <v>0.85</v>
@@ -8401,7 +8406,7 @@
         <v>39</v>
       </c>
       <c r="E279">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="G279">
         <v>0.85</v>
@@ -8424,7 +8429,7 @@
         <v>39</v>
       </c>
       <c r="E280">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="G280">
         <v>0.85</v>
@@ -8447,7 +8452,7 @@
         <v>39</v>
       </c>
       <c r="E281">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="G281">
         <v>0.85</v>
@@ -8470,7 +8475,7 @@
         <v>39</v>
       </c>
       <c r="E282">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="G282">
         <v>0.85</v>
@@ -8493,7 +8498,7 @@
         <v>39</v>
       </c>
       <c r="E283">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="G283">
         <v>0.85</v>
@@ -8516,7 +8521,7 @@
         <v>39</v>
       </c>
       <c r="E284">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="G284">
         <v>0.85</v>
@@ -8539,7 +8544,7 @@
         <v>39</v>
       </c>
       <c r="E285">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="G285">
         <v>0.85</v>
@@ -8562,7 +8567,7 @@
         <v>39</v>
       </c>
       <c r="E286">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G286">
         <v>0.85</v>
@@ -8585,7 +8590,7 @@
         <v>39</v>
       </c>
       <c r="E287">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G287">
         <v>0.85</v>
@@ -8602,16 +8607,16 @@
         <v>41</v>
       </c>
       <c r="C288" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D288" t="s">
         <v>39</v>
       </c>
       <c r="E288">
-        <v>1990</v>
+        <v>2018</v>
       </c>
       <c r="G288">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="I288" t="s">
         <v>49</v>
@@ -8625,16 +8630,16 @@
         <v>41</v>
       </c>
       <c r="C289" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D289" t="s">
         <v>39</v>
       </c>
       <c r="E289">
-        <v>1991</v>
+        <v>2019</v>
       </c>
       <c r="G289">
-        <v>0.1</v>
+        <v>0.85</v>
       </c>
       <c r="I289" t="s">
         <v>49</v>
@@ -8654,10 +8659,10 @@
         <v>39</v>
       </c>
       <c r="E290">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="G290">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I290" t="s">
         <v>49</v>
@@ -8677,7 +8682,7 @@
         <v>39</v>
       </c>
       <c r="E291">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="G291">
         <v>0.1</v>
@@ -8700,7 +8705,7 @@
         <v>39</v>
       </c>
       <c r="E292">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="G292">
         <v>0.1</v>
@@ -8723,7 +8728,7 @@
         <v>39</v>
       </c>
       <c r="E293">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="G293">
         <v>0.1</v>
@@ -8746,7 +8751,7 @@
         <v>39</v>
       </c>
       <c r="E294">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="G294">
         <v>0.1</v>
@@ -8769,7 +8774,7 @@
         <v>39</v>
       </c>
       <c r="E295">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="G295">
         <v>0.1</v>
@@ -8792,7 +8797,7 @@
         <v>39</v>
       </c>
       <c r="E296">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="G296">
         <v>0.1</v>
@@ -8815,7 +8820,7 @@
         <v>39</v>
       </c>
       <c r="E297">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="G297">
         <v>0.1</v>
@@ -8838,7 +8843,7 @@
         <v>39</v>
       </c>
       <c r="E298">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="G298">
         <v>0.1</v>
@@ -8861,7 +8866,7 @@
         <v>39</v>
       </c>
       <c r="E299">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="G299">
         <v>0.1</v>
@@ -8884,7 +8889,7 @@
         <v>39</v>
       </c>
       <c r="E300">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="G300">
         <v>0.1</v>
@@ -8907,7 +8912,7 @@
         <v>39</v>
       </c>
       <c r="E301">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="G301">
         <v>0.1</v>
@@ -8930,7 +8935,7 @@
         <v>39</v>
       </c>
       <c r="E302">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="G302">
         <v>0.1</v>
@@ -8953,7 +8958,7 @@
         <v>39</v>
       </c>
       <c r="E303">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="G303">
         <v>0.1</v>
@@ -8976,7 +8981,7 @@
         <v>39</v>
       </c>
       <c r="E304">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="G304">
         <v>0.1</v>
@@ -8999,7 +9004,7 @@
         <v>39</v>
       </c>
       <c r="E305">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="G305">
         <v>0.1</v>
@@ -9022,7 +9027,7 @@
         <v>39</v>
       </c>
       <c r="E306">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="G306">
         <v>0.1</v>
@@ -9045,7 +9050,7 @@
         <v>39</v>
       </c>
       <c r="E307">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="G307">
         <v>0.1</v>
@@ -9068,7 +9073,7 @@
         <v>39</v>
       </c>
       <c r="E308">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="G308">
         <v>0.1</v>
@@ -9091,7 +9096,7 @@
         <v>39</v>
       </c>
       <c r="E309">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="G309">
         <v>0.1</v>
@@ -9114,7 +9119,7 @@
         <v>39</v>
       </c>
       <c r="E310">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="G310">
         <v>0.1</v>
@@ -9137,7 +9142,7 @@
         <v>39</v>
       </c>
       <c r="E311">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="G311">
         <v>0.1</v>
@@ -9160,7 +9165,7 @@
         <v>39</v>
       </c>
       <c r="E312">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="G312">
         <v>0.1</v>
@@ -9183,7 +9188,7 @@
         <v>39</v>
       </c>
       <c r="E313">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="G313">
         <v>0.1</v>
@@ -9206,7 +9211,7 @@
         <v>39</v>
       </c>
       <c r="E314">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="G314">
         <v>0.1</v>
@@ -9229,7 +9234,7 @@
         <v>39</v>
       </c>
       <c r="E315">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="G315">
         <v>0.1</v>
@@ -9252,7 +9257,7 @@
         <v>39</v>
       </c>
       <c r="E316">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G316">
         <v>0.1</v>
@@ -9275,7 +9280,7 @@
         <v>39</v>
       </c>
       <c r="E317">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="G317">
         <v>0.1</v>
@@ -9284,14 +9289,60 @@
         <v>49</v>
       </c>
     </row>
-    <row r="430" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K430" s="2"/>
+    <row r="318" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>16</v>
+      </c>
+      <c r="B318" t="s">
+        <v>41</v>
+      </c>
+      <c r="C318" t="s">
+        <v>29</v>
+      </c>
+      <c r="D318" t="s">
+        <v>39</v>
+      </c>
+      <c r="E318">
+        <v>2018</v>
+      </c>
+      <c r="G318">
+        <v>0.1</v>
+      </c>
+      <c r="I318" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="319" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>16</v>
+      </c>
+      <c r="B319" t="s">
+        <v>41</v>
+      </c>
+      <c r="C319" t="s">
+        <v>29</v>
+      </c>
+      <c r="D319" t="s">
+        <v>39</v>
+      </c>
+      <c r="E319">
+        <v>2019</v>
+      </c>
+      <c r="G319">
+        <v>0.1</v>
+      </c>
+      <c r="I319" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="432" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K432" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:L850" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A5:L852" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K258" r:id="rId1" xr:uid="{F4373F22-5F19-834C-83D0-AE7B39FD63BE}"/>
+    <hyperlink ref="K260" r:id="rId1" xr:uid="{F4373F22-5F19-834C-83D0-AE7B39FD63BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>